<commit_message>
changes to media file
changes to media file
</commit_message>
<xml_diff>
--- a/src/Files/barret_import5.0.xlsx
+++ b/src/Files/barret_import5.0.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelnkollo/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelnkollo/Documents/GitHub/Innova2/InnovaRegression/src/Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{782FFCC4-1EBE-3D4D-BA2F-4A8E4340EB95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5F97292-3A26-5347-9EA5-8C5BB00F0F8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="39200" yWindow="6100" windowWidth="35840" windowHeight="20480" tabRatio="988" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="50">
   <si>
     <t>Year</t>
   </si>
@@ -264,7 +264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -285,20 +285,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -617,7 +603,7 @@
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:N21"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -628,7 +614,7 @@
     <col min="4" max="4" width="23.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.5" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.5" style="1" bestFit="1" customWidth="1"/>
@@ -657,7 +643,7 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
@@ -682,39 +668,38 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="9">
+    <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
         <v>1976</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="1">
         <v>1</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9">
+      <c r="K2" s="1">
         <v>190000</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="M2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="N2" s="13" t="s">
+      <c r="N2" s="7" t="s">
         <v>42</v>
       </c>
     </row>
@@ -737,13 +722,13 @@
       <c r="F3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K3" s="1">
         <v>385000</v>
       </c>
-      <c r="L3" s="9" t="s">
+      <c r="L3" s="1" t="s">
         <v>49</v>
       </c>
       <c r="M3" s="6" t="s">
@@ -772,13 +757,13 @@
       <c r="F4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K4" s="1">
         <v>275000</v>
       </c>
-      <c r="L4" s="9" t="s">
+      <c r="L4" s="1" t="s">
         <v>49</v>
       </c>
       <c r="M4" s="6" t="s">
@@ -807,13 +792,13 @@
       <c r="F5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K5" s="1">
         <v>6600</v>
       </c>
-      <c r="L5" s="9" t="s">
+      <c r="L5" s="1" t="s">
         <v>49</v>
       </c>
       <c r="M5" s="6" t="s">
@@ -842,13 +827,13 @@
       <c r="F6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K6" s="1">
         <v>4070</v>
       </c>
-      <c r="L6" s="9" t="s">
+      <c r="L6" s="1" t="s">
         <v>49</v>
       </c>
       <c r="M6" s="6" t="s">
@@ -877,13 +862,13 @@
       <c r="F7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K7" s="1">
         <v>12650</v>
       </c>
-      <c r="L7" s="9" t="s">
+      <c r="L7" s="1" t="s">
         <v>49</v>
       </c>
       <c r="M7" s="6" t="s">
@@ -912,13 +897,13 @@
       <c r="F8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K8" s="1">
         <v>85000</v>
       </c>
-      <c r="L8" s="9" t="s">
+      <c r="L8" s="1" t="s">
         <v>49</v>
       </c>
       <c r="M8" s="6" t="s">
@@ -929,78 +914,95 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D9" s="4"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="7"/>
+      <c r="A9" s="1">
+        <v>1962</v>
+      </c>
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="1">
+        <v>7</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K9" s="1">
+        <v>85000</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="N9" s="7" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L10" s="9"/>
       <c r="M10" s="6"/>
       <c r="N10" s="7"/>
     </row>
     <row r="11" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D11" s="4"/>
-      <c r="L11" s="9"/>
       <c r="M11" s="6"/>
       <c r="N11" s="7"/>
     </row>
     <row r="12" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D12" s="4"/>
-      <c r="L12" s="9"/>
       <c r="M12" s="6"/>
       <c r="N12" s="7"/>
     </row>
     <row r="13" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L13" s="9"/>
       <c r="M13" s="6"/>
       <c r="N13" s="7"/>
     </row>
     <row r="14" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D14" s="4"/>
-      <c r="L14" s="9"/>
       <c r="M14" s="6"/>
       <c r="N14" s="7"/>
     </row>
     <row r="15" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D15" s="4"/>
-      <c r="L15" s="9"/>
       <c r="M15" s="6"/>
       <c r="N15" s="7"/>
     </row>
     <row r="16" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
-      <c r="L16" s="9"/>
       <c r="M16" s="6"/>
       <c r="N16" s="7"/>
     </row>
     <row r="17" spans="4:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D17" s="4"/>
-      <c r="L17" s="9"/>
       <c r="M17" s="6"/>
       <c r="N17" s="7"/>
     </row>
     <row r="18" spans="4:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D18" s="4"/>
-      <c r="L18" s="9"/>
       <c r="M18" s="6"/>
       <c r="N18" s="7"/>
     </row>
     <row r="19" spans="4:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L19" s="9"/>
       <c r="M19" s="6"/>
       <c r="N19" s="7"/>
     </row>
     <row r="20" spans="4:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D20" s="4"/>
-      <c r="L20" s="9"/>
       <c r="M20" s="6"/>
       <c r="N20" s="7"/>
     </row>
     <row r="21" spans="4:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D21" s="4"/>
-      <c r="L21" s="9"/>
       <c r="M21" s="6"/>
       <c r="N21" s="7"/>
     </row>
@@ -1012,6 +1014,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002AB7E647B08EEE4DB6CCAE340B6DD4B3" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="712b19e888fe442f1622d5ec33115fa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fe0145de-900b-49a2-ae7f-d8772a1daa2f" xmlns:ns3="8e1abdca-e57e-4263-b850-c61e1bbfd414" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0e7d88bcd397f4de1ea40e6c8c3b9d72" ns2:_="" ns3:_="">
     <xsd:import namespace="fe0145de-900b-49a2-ae7f-d8772a1daa2f"/>
@@ -1234,22 +1251,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4264EE18-3DB7-4B74-AC4E-F45B10D664E8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3DDB17AB-1028-47ED-9564-C4B259D960F2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45C76E89-86BC-4803-A8E0-FFDFA07ADA29}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1266,21 +1285,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3DDB17AB-1028-47ED-9564-C4B259D960F2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4264EE18-3DB7-4B74-AC4E-F45B10D664E8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>